<commit_message>
Add minor alignments of Kew_2019_2 custom code with previous Kew datasets
</commit_message>
<xml_diff>
--- a/data/Kew_2019_1/raw/source_dois.xlsx
+++ b/data/Kew_2019_1/raw/source_dois.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208613_ad_unsw_edu_au/Documents/RA Work/AusTraits/austraits.build/data/Kew_2019_1/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_F25DC773A252ABDACC10484FF9DC7E805ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B62FE8C-80DF-42CD-A1D9-D11098BD8D40}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC10484FF9DC7E805ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5ED20461-3B95-4C00-A9CC-264C0F50C611}"/>
   <bookViews>
-    <workbookView xWindow="10005" yWindow="1980" windowWidth="21600" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="2115" windowWidth="21600" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>source</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>https://ucjeps.berkeley.edu/baker/</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/S1146-609X(00)01084-5</t>
+  </si>
+  <si>
+    <t>PérezFernández_2000</t>
   </si>
 </sst>
 </file>
@@ -89,6 +95,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,7 +388,16 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>